<commit_message>
added work in bulk
</commit_message>
<xml_diff>
--- a/resources/raja.xlsx
+++ b/resources/raja.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="126">
   <si>
     <t>Nom</t>
   </si>
@@ -235,15 +235,9 @@
     <t>Nouveaux produits</t>
   </si>
   <si>
-    <t>Charge en kg</t>
-  </si>
-  <si>
     <t>Type de fermeture</t>
   </si>
   <si>
-    <t>Epaisseur(en micro)</t>
-  </si>
-  <si>
     <t>Adapté au contact alimentaire</t>
   </si>
   <si>
@@ -295,9 +289,6 @@
     <t>Pastilles et étiquettes de signalisation biosourcées, recyclées, recyclables</t>
   </si>
   <si>
-    <t>AGIPA</t>
-  </si>
-  <si>
     <t>papier</t>
   </si>
   <si>
@@ -404,6 +395,9 @@
   </si>
   <si>
     <t>goal_name</t>
+  </si>
+  <si>
+    <t>Epaisseur (en micro)</t>
   </si>
 </sst>
 </file>
@@ -779,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -986,10 +980,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,19 +993,18 @@
     <col min="6" max="6" width="41.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="67.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D1" t="s">
         <v>59</v>
@@ -1053,146 +1046,139 @@
         <v>71</v>
       </c>
       <c r="Q1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" t="s">
         <v>72</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>73</v>
       </c>
-      <c r="S1" t="s">
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="T1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D2" s="1">
         <v>58.3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>114004</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D3" s="2">
         <v>5.46</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1">
         <v>258</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -1201,32 +1187,31 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1">
         <v>16.149999999999999</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1234,71 +1219,69 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1" t="s">
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="D6" s="1">
         <v>1.91</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1" t="s">
-        <v>119</v>
+      <c r="S6" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>